<commit_message>
Apothecarius Integration - AIChip crafting
medical system of apothecarius fully implemented also added ai chip
crafting and a bit of balancing
</commit_message>
<xml_diff>
--- a/Superior Crafting.xlsx
+++ b/Superior Crafting.xlsx
@@ -1847,6 +1847,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1864,9 +1867,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -12630,57 +12630,57 @@
       <c r="A52" s="21"/>
       <c r="B52" s="21"/>
       <c r="C52" s="21"/>
-      <c r="D52" s="42" t="s">
+      <c r="D52" s="36" t="s">
         <v>304</v>
       </c>
-      <c r="E52" s="42"/>
-      <c r="F52" s="42"/>
-      <c r="G52" s="42"/>
-      <c r="H52" s="42"/>
+      <c r="E52" s="36"/>
+      <c r="F52" s="36"/>
+      <c r="G52" s="36"/>
+      <c r="H52" s="36"/>
       <c r="I52" s="22"/>
     </row>
     <row r="53" spans="1:9" ht="15" customHeight="1">
       <c r="A53" s="21"/>
       <c r="B53" s="21"/>
       <c r="C53" s="21"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
-      <c r="F53" s="42"/>
-      <c r="G53" s="42"/>
-      <c r="H53" s="42"/>
+      <c r="D53" s="36"/>
+      <c r="E53" s="36"/>
+      <c r="F53" s="36"/>
+      <c r="G53" s="36"/>
+      <c r="H53" s="36"/>
       <c r="I53" s="22"/>
     </row>
     <row r="54" spans="1:9" ht="15" customHeight="1">
       <c r="A54" s="21"/>
       <c r="B54" s="21"/>
       <c r="C54" s="21"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="42"/>
-      <c r="F54" s="42"/>
-      <c r="G54" s="42"/>
-      <c r="H54" s="42"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="36"/>
+      <c r="F54" s="36"/>
+      <c r="G54" s="36"/>
+      <c r="H54" s="36"/>
       <c r="I54" s="22"/>
     </row>
     <row r="55" spans="1:9" ht="15" customHeight="1">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="21"/>
-      <c r="D55" s="42"/>
-      <c r="E55" s="42"/>
-      <c r="F55" s="42"/>
-      <c r="G55" s="42"/>
-      <c r="H55" s="42"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
+      <c r="F55" s="36"/>
+      <c r="G55" s="36"/>
+      <c r="H55" s="36"/>
       <c r="I55" s="22"/>
     </row>
     <row r="56" spans="1:9" ht="15" customHeight="1">
       <c r="A56" s="21"/>
       <c r="B56" s="21"/>
       <c r="C56" s="21"/>
-      <c r="D56" s="42"/>
-      <c r="E56" s="42"/>
-      <c r="F56" s="42"/>
-      <c r="G56" s="42"/>
-      <c r="H56" s="42"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="36"/>
+      <c r="F56" s="36"/>
+      <c r="G56" s="36"/>
+      <c r="H56" s="36"/>
       <c r="I56" s="22"/>
     </row>
     <row r="57" spans="1:9">
@@ -13386,37 +13386,37 @@
       <c r="L1" s="44"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="37" t="s">
         <v>408</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="38" t="s">
         <v>415</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="38" t="s">
         <v>416</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="38" t="s">
         <v>418</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="38" t="s">
         <v>417</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="38" t="s">
         <v>419</v>
       </c>
-      <c r="H2" s="38" t="s">
+      <c r="H2" s="39" t="s">
         <v>420</v>
       </c>
-      <c r="I2" s="39" t="s">
+      <c r="I2" s="40" t="s">
         <v>423</v>
       </c>
       <c r="J2" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="K2" s="40" t="s">
+      <c r="K2" s="41" t="s">
         <v>428</v>
       </c>
       <c r="L2" s="33" t="s">
@@ -13571,7 +13571,7 @@
       <c r="K6" s="1">
         <v>0</v>
       </c>
-      <c r="L6" s="41">
+      <c r="L6" s="42">
         <v>1</v>
       </c>
     </row>
@@ -13592,37 +13592,37 @@
       <c r="L7" s="44"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="37" t="s">
         <v>408</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="38" t="s">
         <v>415</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="38" t="s">
         <v>416</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="38" t="s">
         <v>418</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="38" t="s">
         <v>417</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G8" s="38" t="s">
         <v>419</v>
       </c>
-      <c r="H8" s="38" t="s">
+      <c r="H8" s="39" t="s">
         <v>420</v>
       </c>
-      <c r="I8" s="39" t="s">
+      <c r="I8" s="40" t="s">
         <v>423</v>
       </c>
       <c r="J8" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="K8" s="40" t="s">
+      <c r="K8" s="41" t="s">
         <v>428</v>
       </c>
       <c r="L8" s="33" t="s">
@@ -13663,7 +13663,7 @@
       <c r="K9" s="1">
         <v>0</v>
       </c>
-      <c r="L9" s="41">
+      <c r="L9" s="42">
         <v>1</v>
       </c>
     </row>
@@ -13701,7 +13701,7 @@
       <c r="K10" s="1">
         <v>0</v>
       </c>
-      <c r="L10" s="41">
+      <c r="L10" s="42">
         <v>1</v>
       </c>
     </row>
@@ -13739,7 +13739,7 @@
       <c r="K11" s="1">
         <v>0</v>
       </c>
-      <c r="L11" s="41">
+      <c r="L11" s="42">
         <v>1</v>
       </c>
     </row>
@@ -13777,7 +13777,7 @@
       <c r="K12" s="1">
         <v>0</v>
       </c>
-      <c r="L12" s="41">
+      <c r="L12" s="42">
         <v>3</v>
       </c>
     </row>
@@ -13815,7 +13815,7 @@
       <c r="K13" s="1">
         <v>135</v>
       </c>
-      <c r="L13" s="41">
+      <c r="L13" s="42">
         <v>1</v>
       </c>
     </row>
@@ -13853,7 +13853,7 @@
       <c r="K14" s="1">
         <v>0</v>
       </c>
-      <c r="L14" s="41">
+      <c r="L14" s="42">
         <v>4</v>
       </c>
     </row>
@@ -13891,7 +13891,7 @@
       <c r="K15" s="1">
         <v>0</v>
       </c>
-      <c r="L15" s="41">
+      <c r="L15" s="42">
         <v>1</v>
       </c>
     </row>
@@ -13929,7 +13929,7 @@
       <c r="K16" s="1">
         <v>0</v>
       </c>
-      <c r="L16" s="41">
+      <c r="L16" s="42">
         <v>1</v>
       </c>
     </row>
@@ -13967,7 +13967,7 @@
       <c r="K17" s="1">
         <v>0</v>
       </c>
-      <c r="L17" s="41">
+      <c r="L17" s="42">
         <v>3</v>
       </c>
     </row>
@@ -13988,37 +13988,37 @@
       <c r="L18" s="44"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="37" t="s">
         <v>408</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="38" t="s">
         <v>415</v>
       </c>
-      <c r="D19" s="37" t="s">
+      <c r="D19" s="38" t="s">
         <v>416</v>
       </c>
-      <c r="E19" s="37" t="s">
+      <c r="E19" s="38" t="s">
         <v>418</v>
       </c>
-      <c r="F19" s="37" t="s">
+      <c r="F19" s="38" t="s">
         <v>417</v>
       </c>
-      <c r="G19" s="37" t="s">
+      <c r="G19" s="38" t="s">
         <v>419</v>
       </c>
-      <c r="H19" s="38" t="s">
+      <c r="H19" s="39" t="s">
         <v>420</v>
       </c>
-      <c r="I19" s="39" t="s">
+      <c r="I19" s="40" t="s">
         <v>423</v>
       </c>
       <c r="J19" s="33" t="s">
         <v>427</v>
       </c>
-      <c r="K19" s="40" t="s">
+      <c r="K19" s="41" t="s">
         <v>428</v>
       </c>
       <c r="L19" s="33" t="s">

</xml_diff>